<commit_message>
Export with no is_pref and no lev distance
</commit_message>
<xml_diff>
--- a/playlist_per_work/_vry001vrya01.xlsx
+++ b/playlist_per_work/_vry001vrya01.xlsx
@@ -483,19 +483,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>#en</t>
+          <t>#roosje-vasthouwende</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>Roosje vasthouwende</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -509,19 +505,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>#met-een-glas-wyn-in-de-hand</t>
+          <t>#alleen</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>met een glas wyn in de hand</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>alleen</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -535,19 +527,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>#alleen</t>
+          <t>#met-een-glas-wyn-in-de-hand</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>alleen</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>met een glas wyn in de hand</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -561,19 +549,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>#roosje-vasthouwende</t>
+          <t>#en</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Roosje vasthouwende</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>

</xml_diff>